<commit_message>
C02_WriteExcel class'inda calismalar yapildi.
</commit_message>
<xml_diff>
--- a/src/test/java/resources/Capitals.xlsx
+++ b/src/test/java/resources/Capitals.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\OneDrive\Masaüstü\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bahad\IdeaProjects\SeleniumPractices\src\test\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D40DB08-2F6B-449F-9E2B-48E40FB6F0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7900"/>
+    <workbookView xWindow="20370" yWindow="-105" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>COUNTRY</t>
   </si>
@@ -88,24 +89,12 @@
   </si>
   <si>
     <t>NUFUS</t>
-  </si>
-  <si>
-    <t>712816</t>
-  </si>
-  <si>
-    <t>2161000</t>
-  </si>
-  <si>
-    <t>8982000</t>
-  </si>
-  <si>
-    <t>5663000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -147,9 +136,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -364,19 +353,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -387,51 +376,51 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s" s="0">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" t="n" s="0">
+        <v>712816.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s" s="0">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" t="n" s="0">
+        <v>2161000.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s" s="0">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" t="n" s="0">
+        <v>8982000.0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s" s="0">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" t="n" s="0">
+        <v>5.663E8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -439,7 +428,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -447,7 +436,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -455,7 +444,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -463,7 +452,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -471,7 +460,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>

</xml_diff>